<commit_message>
Edit, Delete, Filter by PSA implemented
</commit_message>
<xml_diff>
--- a/sample_data/scse_cz3003_2018_s1_cms_app_publicserviceannouncement.xlsx
+++ b/sample_data/scse_cz3003_2018_s1_cms_app_publicserviceannouncement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HaoDe\Gits\scse_cz3003_2018_s1_cms\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{611BC059-42E0-4EDD-989D-DA6F635546D1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1059D960-5933-42E6-B670-92B508331E94}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10380" xr2:uid="{6ACC9CDB-377F-4EF5-AE34-D3A838677C0D}"/>
   </bookViews>
@@ -445,7 +445,7 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="b">
+      <c r="D2">
         <v>1</v>
       </c>
     </row>
@@ -459,7 +459,7 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="b">
+      <c r="D3">
         <v>1</v>
       </c>
     </row>
@@ -473,7 +473,7 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="b">
+      <c r="D4">
         <v>1</v>
       </c>
     </row>

</xml_diff>